<commit_message>
added ffort benchmark set; DFT convertor
</commit_message>
<xml_diff>
--- a/models/ctmc/cluster/parameters.xlsx
+++ b/models/ctmc/cluster/parameters.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -37,24 +36,6 @@
     <t>gaussian</t>
   </si>
   <si>
-    <t>property</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>P=? [ F&lt;=2000 !"minimum" ]</t>
-  </si>
-  <si>
-    <t>R{"num_repairs"}=? [ C&lt;=2000 ]</t>
-  </si>
-  <si>
-    <t>Prob. that QoS drops below min. quality before time T=2000</t>
-  </si>
-  <si>
-    <t>Exp. number of repairs by time T=2000</t>
-  </si>
-  <si>
     <t>ws_fail</t>
   </si>
   <si>
@@ -65,9 +46,6 @@
   </si>
   <si>
     <t>inverse</t>
-  </si>
-  <si>
-    <t>enabled</t>
   </si>
 </sst>
 </file>
@@ -387,7 +365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -407,12 +385,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -429,7 +407,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -446,7 +424,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -458,58 +436,6 @@
         <v>30</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="50.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parameter changes in SIR model
</commit_message>
<xml_diff>
--- a/models/ctmc/cluster/parameters.xlsx
+++ b/models/ctmc/cluster/parameters.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -27,15 +27,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>gaussian</t>
-  </si>
-  <si>
     <t>ws_fail</t>
   </si>
   <si>
@@ -46,6 +37,24 @@
   </si>
   <si>
     <t>inverse</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>ub</t>
+  </si>
+  <si>
+    <t>ws_check</t>
+  </si>
+  <si>
+    <t>ws_repair</t>
+  </si>
+  <si>
+    <t>switch_check</t>
   </si>
 </sst>
 </file>
@@ -363,13 +372,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -379,64 +391,115 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>500</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>4000</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>1.25E-3</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>5000</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>1E-3</v>
       </c>
       <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>